<commit_message>
Added Code For Date Selection For WFMTimeCardTotal Test
</commit_message>
<xml_diff>
--- a/Data/Timecard_Total_Amy2.xlsx
+++ b/Data/Timecard_Total_Amy2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4303B511-4F2A-4B2F-A062-68E4D61C3419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Tabelle1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>EmpID</t>
   </si>
@@ -26,6 +25,12 @@
     <t>Paycode</t>
   </si>
   <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
     <t>TestResult</t>
   </si>
   <si>
@@ -35,7 +40,13 @@
     <t>SK- Total Worked Hours</t>
   </si>
   <si>
-    <t>Passed</t>
+    <t>01/10/2024</t>
+  </si>
+  <si>
+    <t>10/11/2024</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
   <si>
     <t>95:00</t>
@@ -44,58 +55,67 @@
     <t>SK- Worked Hours and HOL Unwrkd</t>
   </si>
   <si>
+    <t>14/11/2024</t>
+  </si>
+  <si>
+    <t>178:15</t>
+  </si>
+  <si>
     <t>SK-Tracking Quaterly Hours</t>
-  </si>
-  <si>
-    <t>178:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <color rgb="FFCE9178"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color rgb="FFCE9178"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
+      <color indexed="8"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
+      <color indexed="8"/>
+      <family val="2"/>
       <sz val="12"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
+      <color rgb="FF00B050"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -120,9 +141,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -131,7 +153,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -145,7 +167,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -424,22 +446,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,65 +476,83 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" ht="14.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>10648929</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" ht="14.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>10648915</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10649095</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1 D3:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="F1 F3:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"""Failed"""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Code For Date Selection  Test under  CommonPages in CurrentPayPeriodPage
</commit_message>
<xml_diff>
--- a/Data/Timecard_Total_Amy2.xlsx
+++ b/Data/Timecard_Total_Amy2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>EmpID</t>
   </si>
@@ -450,7 +450,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
@@ -518,6 +518,9 @@
       </c>
       <c r="E3" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
       <c r="G3" s="7"/>
     </row>

</xml_diff>

<commit_message>
code added for PucnhInout
</commit_message>
<xml_diff>
--- a/Data/Timecard_Total_Amy2.xlsx
+++ b/Data/Timecard_Total_Amy2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4303B511-4F2A-4B2F-A062-68E4D61C3419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Tabelle1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>EmpID</t>
   </si>
@@ -26,6 +25,12 @@
     <t>Paycode</t>
   </si>
   <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
     <t>TestResult</t>
   </si>
   <si>
@@ -35,7 +40,13 @@
     <t>SK- Total Worked Hours</t>
   </si>
   <si>
-    <t>Passed</t>
+    <t>01/10/2024</t>
+  </si>
+  <si>
+    <t>10/11/2024</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
   <si>
     <t>95:00</t>
@@ -44,58 +55,67 @@
     <t>SK- Worked Hours and HOL Unwrkd</t>
   </si>
   <si>
+    <t>14/11/2024</t>
+  </si>
+  <si>
+    <t>178:15</t>
+  </si>
+  <si>
     <t>SK-Tracking Quaterly Hours</t>
-  </si>
-  <si>
-    <t>178:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <color rgb="FFCE9178"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color rgb="FFCE9178"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
+      <color indexed="8"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
+      <color indexed="8"/>
+      <family val="2"/>
       <sz val="12"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
+      <color rgb="FF00B050"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -120,9 +141,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -131,7 +153,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -145,7 +167,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -424,22 +446,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,65 +476,83 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" ht="14.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>10648929</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" ht="14.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>10648915</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10649095</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1 D3:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="F1 F3:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"""Failed"""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added DataView & SignOFF Testcase Code
</commit_message>
<xml_diff>
--- a/Data/Timecard_Total_Amy2.xlsx
+++ b/Data/Timecard_Total_Amy2.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DC2749-04F8-4767-A6DD-710D50877446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Tabelle1" state="visible" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -67,41 +68,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
       <family val="3"/>
-      <sz val="11"/>
-      <name val="Consolas"/>
     </font>
     <font>
+      <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Consolas"/>
       <family val="3"/>
-      <sz val="11"/>
-      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="3">
@@ -153,7 +154,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -167,7 +168,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -446,14 +447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
@@ -463,7 +464,7 @@
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="14.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>10648929</v>
       </c>
@@ -503,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="14.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>10648915</v>
       </c>
@@ -521,7 +522,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10649095</v>
       </c>
@@ -540,7 +541,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1 F3:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"""Failed"""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
@@ -548,11 +549,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>